<commit_message>
perbaikan c45 ke 6
</commit_message>
<xml_diff>
--- a/asset/Book2.xlsx
+++ b/asset/Book2.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="21">
   <si>
     <t>NO</t>
   </si>
@@ -461,10 +461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -709,6 +709,214 @@
         <v>6</v>
       </c>
       <c r="H9" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3">
+        <v>2020804139</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3">
+        <v>2020804179</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3">
+        <v>2020434179</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3">
+        <v>2020434179</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3">
+        <v>2020804139</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="3">
+        <v>2020804179</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="3">
+        <v>2020434179</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="3">
+        <v>2020434179</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H17" s="2" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>